<commit_message>
Graficas de error de resistencias
</commit_message>
<xml_diff>
--- a/matlab_ubol/voltajes_resistencias/comp_med.xlsx
+++ b/matlab_ubol/voltajes_resistencias/comp_med.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop_old\proyecto_ubolometro\matlab_ubol\voltajes_resistencias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AE9A72-1840-4366-B1FE-AB6F6D78190D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0880B0D9-31A2-4F94-BD60-09989898AB36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8D965064-6EDB-4D75-9448-C5FBC6AAAC5F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D965064-6EDB-4D75-9448-C5FBC6AAAC5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>Vmuxrows</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>proto chico</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Rmuxr</t>
+  </si>
+  <si>
+    <t>Rmuxc</t>
+  </si>
+  <si>
+    <t>Rtr</t>
   </si>
 </sst>
 </file>
@@ -87,12 +99,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -115,9 +139,23 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,41 +490,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D65122-5141-4BF4-AF1B-2CB7C6405213}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -496,7 +546,7 @@
       <c r="C3" s="2">
         <v>4.1200000000000001E-2</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="8">
         <v>0.25800000000000001</v>
       </c>
       <c r="E3" s="2">
@@ -505,8 +555,24 @@
       <c r="F3" s="1">
         <v>2.66</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="7">
+        <f>F3/10000</f>
+        <v>2.6600000000000001E-4</v>
+      </c>
+      <c r="H3" s="9">
+        <f>C3/G3</f>
+        <v>154.88721804511277</v>
+      </c>
+      <c r="I3" s="9">
+        <f>E3/G3</f>
+        <v>163.9097744360902</v>
+      </c>
+      <c r="J3" s="9">
+        <f>D3/G3</f>
+        <v>969.92481203007515</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -516,7 +582,7 @@
       <c r="C4" s="2">
         <v>3.5499999999999997E-2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="8">
         <v>0.64700000000000002</v>
       </c>
       <c r="E4" s="2">
@@ -525,8 +591,24 @@
       <c r="F4" s="1">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:G6" si="0">F4/10000</f>
+        <v>2.2999999999999998E-4</v>
+      </c>
+      <c r="H4" s="9">
+        <f t="shared" ref="H4:H6" si="1">C4/G4</f>
+        <v>154.34782608695653</v>
+      </c>
+      <c r="I4" s="9">
+        <f t="shared" ref="I4:I6" si="2">E4/G4</f>
+        <v>143.47826086956525</v>
+      </c>
+      <c r="J4" s="9">
+        <f t="shared" ref="J4:J6" si="3">D4/G4</f>
+        <v>2813.04347826087</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -536,7 +618,7 @@
       <c r="C5" s="2">
         <v>3.2300000000000002E-2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="8">
         <v>0.85499999999999998</v>
       </c>
       <c r="E5" s="2">
@@ -545,8 +627,24 @@
       <c r="F5" s="1">
         <v>2.09</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="7">
+        <f t="shared" si="0"/>
+        <v>2.0899999999999998E-4</v>
+      </c>
+      <c r="H5" s="9">
+        <f t="shared" si="1"/>
+        <v>154.54545454545456</v>
+      </c>
+      <c r="I5" s="9">
+        <f t="shared" si="2"/>
+        <v>139.23444976076556</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" si="3"/>
+        <v>4090.909090909091</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -556,7 +654,7 @@
       <c r="C6" s="2">
         <v>3.0300000000000001E-2</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="8">
         <v>0.99099999999999999</v>
       </c>
       <c r="E6" s="2">
@@ -565,34 +663,62 @@
       <c r="F6" s="1">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="G6" s="7">
+        <f t="shared" si="0"/>
+        <v>1.9599999999999999E-4</v>
+      </c>
+      <c r="H6" s="9">
+        <f t="shared" si="1"/>
+        <v>154.59183673469389</v>
+      </c>
+      <c r="I6" s="9">
+        <f t="shared" si="2"/>
+        <v>136.73469387755102</v>
+      </c>
+      <c r="J6" s="9">
+        <f t="shared" si="3"/>
+        <v>5056.1224489795923</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -602,17 +728,33 @@
       <c r="C10" s="2">
         <v>3.8600000000000002E-2</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="8">
         <v>0.28100000000000003</v>
       </c>
       <c r="E10" s="2">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="F10" s="1">
-        <v>2.57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.65</v>
+      </c>
+      <c r="G10" s="7">
+        <f>F10/10000</f>
+        <v>2.6499999999999999E-4</v>
+      </c>
+      <c r="H10" s="9">
+        <f>C10/G10</f>
+        <v>145.66037735849059</v>
+      </c>
+      <c r="I10" s="9">
+        <f>E10/G10</f>
+        <v>132.07547169811323</v>
+      </c>
+      <c r="J10" s="9">
+        <f>D10/G10</f>
+        <v>1060.3773584905662</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -622,7 +764,7 @@
       <c r="C11" s="2">
         <v>3.4299999999999997E-2</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="8">
         <v>0.74</v>
       </c>
       <c r="E11" s="2">
@@ -631,8 +773,24 @@
       <c r="F11" s="1">
         <v>2.21</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="7">
+        <f t="shared" ref="G11:G13" si="4">F11/10000</f>
+        <v>2.2100000000000001E-4</v>
+      </c>
+      <c r="H11" s="9">
+        <f t="shared" ref="H11:H13" si="5">C11/G11</f>
+        <v>155.20361990950224</v>
+      </c>
+      <c r="I11" s="9">
+        <f t="shared" ref="I11:I13" si="6">E11/G11</f>
+        <v>140.27149321266967</v>
+      </c>
+      <c r="J11" s="9">
+        <f t="shared" ref="J11:J13" si="7">D11/G11</f>
+        <v>3348.4162895927602</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -642,17 +800,33 @@
       <c r="C12" s="2">
         <v>2.8299999999999999E-2</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="8">
         <v>1.0900000000000001</v>
       </c>
       <c r="E12" s="2">
         <v>2.4799999999999999E-2</v>
       </c>
       <c r="F12" s="1">
-        <v>1.88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.89</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="4"/>
+        <v>1.8899999999999999E-4</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" si="5"/>
+        <v>149.73544973544975</v>
+      </c>
+      <c r="I12" s="9">
+        <f t="shared" si="6"/>
+        <v>131.21693121693121</v>
+      </c>
+      <c r="J12" s="9">
+        <f t="shared" si="7"/>
+        <v>5767.195767195768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -662,7 +836,7 @@
       <c r="C13" s="2">
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="8">
         <v>1.48</v>
       </c>
       <c r="E13" s="2">
@@ -670,6 +844,22 @@
       </c>
       <c r="F13" s="1">
         <v>1.49</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="4"/>
+        <v>1.4899999999999999E-4</v>
+      </c>
+      <c r="H13" s="9">
+        <f t="shared" si="5"/>
+        <v>151.00671140939599</v>
+      </c>
+      <c r="I13" s="9">
+        <f t="shared" si="6"/>
+        <v>141.61073825503357</v>
+      </c>
+      <c r="J13" s="9">
+        <f t="shared" si="7"/>
+        <v>9932.8859060402683</v>
       </c>
     </row>
   </sheetData>

</xml_diff>